<commit_message>
enchainement des methodes des dataframes
</commit_message>
<xml_diff>
--- a/data/chantier.xlsx
+++ b/data/chantier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJETS\POINTAGE\POINTAGE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD2D2D6-F74C-446E-9471-C32A0FD57CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1138D2FE-487C-44DE-9F6D-62E877FBEF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>id_chantier</t>
   </si>
   <si>
     <t>zone</t>
+  </si>
+  <si>
+    <t>abs</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -99,6 +102,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,10 +320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B984"/>
+  <dimension ref="A1:G993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -336,94 +342,201 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>3277</v>
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>1336</v>
+      </c>
+      <c r="B3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>3333</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-    </row>
     <row r="4" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>3401</v>
+      <c r="A4" s="5">
+        <v>3186</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>3427</v>
+      <c r="A5" s="5">
+        <v>3232</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
+        <v>3270</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>3277</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>3333</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>3401</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>3411</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>3414</v>
+      </c>
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>3425</v>
+      </c>
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>3427</v>
+      </c>
+      <c r="B13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>3428</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>3433</v>
+      </c>
+      <c r="B15" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
         <v>3450</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B16" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
         <v>3496</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B17" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1360,9 +1473,18 @@
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
-    <sortCondition ref="A2:A7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
+    <sortCondition ref="A2:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>